<commit_message>
Atualização Controle de Alteração
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Controle_Alteracao.xlsx
+++ b/Documentação/Planilhas/Controle_Alteracao.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="timezone" sheetId="1" r:id="rId1"/>
     <sheet name="sincronizacao versao" sheetId="2" r:id="rId2"/>
     <sheet name="DT_ULT_ATUALIZACAO" sheetId="3" r:id="rId3"/>
+    <sheet name="Alteracao Tabelas" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="250">
   <si>
     <t>RESPONSÁVEL</t>
   </si>
@@ -478,9 +479,6 @@
   </si>
   <si>
     <t>DT_ULTIMA_ATUALIZ_NF</t>
-  </si>
-  <si>
-    <t>DT_STATUS</t>
   </si>
   <si>
     <t>stg_dom_cap_bco_parceiro</t>
@@ -696,13 +694,91 @@
   </si>
   <si>
     <t>não está sendo utilizada, porém o Riccardo pediu para mantermos no banco</t>
+  </si>
+  <si>
+    <t>Nome do Atributo</t>
+  </si>
+  <si>
+    <t>Tipo Alteração</t>
+  </si>
+  <si>
+    <t>VL_FRETE_CLIENTE</t>
+  </si>
+  <si>
+    <t>VL_FRETE_CIA</t>
+  </si>
+  <si>
+    <t>vw_pev_cab</t>
+  </si>
+  <si>
+    <t>Nome da Tabela/view</t>
+  </si>
+  <si>
+    <t>Data da Alteração</t>
+  </si>
+  <si>
+    <t>vw_trp_transporte</t>
+  </si>
+  <si>
+    <t>NR_NOTA_FATURA</t>
+  </si>
+  <si>
+    <t>NR_SERIE_NOTA_FATURA</t>
+  </si>
+  <si>
+    <t>vw_dom_tipo_ordem_venda</t>
+  </si>
+  <si>
+    <t>No projeto SharedDimensionStaging_LN foi inserido um dtsx chamado ods_tipo_ordem_venda. A tabela criada no banco MIS_SHARED_DIMENSION tem o nome de dim.ods_tipo_ordem_venda</t>
+  </si>
+  <si>
+    <t>vw_trp_analitico</t>
+  </si>
+  <si>
+    <t>NR_EXPEDICAO</t>
+  </si>
+  <si>
+    <t>CD_REGIAO_TRANSPORTADORA</t>
+  </si>
+  <si>
+    <t>CD_CIA</t>
+  </si>
+  <si>
+    <t>vw_nfv_eletronica</t>
+  </si>
+  <si>
+    <t>vw_nfv_cab</t>
+  </si>
+  <si>
+    <t>NR_NF_FATURA</t>
+  </si>
+  <si>
+    <t>NR_NF_REMESSA</t>
+  </si>
+  <si>
+    <t>Na view, fizemos a conversão para texto (to_char)</t>
+  </si>
+  <si>
+    <t>na view, retiramos a função ABS</t>
+  </si>
+  <si>
+    <t>na view, substituimos no else de 0 por null</t>
+  </si>
+  <si>
+    <t>na view, substituimos no else de " " por null</t>
+  </si>
+  <si>
+    <t>retirado da view e tabela</t>
+  </si>
+  <si>
+    <t>inserido na view e tabela</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -748,6 +824,19 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -854,7 +943,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -931,11 +1020,160 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1215,27 +1453,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A1:M59" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:M59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A1:M58" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A1:M58">
     <filterColumn colId="3"/>
     <filterColumn colId="4"/>
     <filterColumn colId="5"/>
     <filterColumn colId="12"/>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" name="tabela" dataDxfId="12"/>
-    <tableColumn id="2" name="nome_campo_x000a_ (DE)" dataDxfId="11"/>
-    <tableColumn id="3" name="nome_campo0 _x000a_(PARA)" dataDxfId="10"/>
-    <tableColumn id="12" name="GitHub" dataDxfId="9"/>
-    <tableColumn id="10" name="Mapeamento_Stage_LN" dataDxfId="8"/>
-    <tableColumn id="11" name="Mapeamento_ODS_LN" dataDxfId="7"/>
-    <tableColumn id="4" name="MIS_MIGRACAO _x000a_201" dataDxfId="6"/>
-    <tableColumn id="5" name="MIS_MIGRACAO _x000a_301" dataDxfId="5"/>
-    <tableColumn id="6" name="MIS_ODS" dataDxfId="4"/>
-    <tableColumn id="7" name="Views _x000a_Oracle" dataDxfId="3"/>
-    <tableColumn id="8" name="SSIS's" dataDxfId="2"/>
-    <tableColumn id="9" name="Data de Correção" dataDxfId="1"/>
-    <tableColumn id="13" name="Observação" dataDxfId="0"/>
+    <tableColumn id="1" name="tabela" dataDxfId="19"/>
+    <tableColumn id="2" name="nome_campo_x000a_ (DE)" dataDxfId="18"/>
+    <tableColumn id="3" name="nome_campo0 _x000a_(PARA)" dataDxfId="17"/>
+    <tableColumn id="12" name="GitHub" dataDxfId="16"/>
+    <tableColumn id="10" name="Mapeamento_Stage_LN" dataDxfId="15"/>
+    <tableColumn id="11" name="Mapeamento_ODS_LN" dataDxfId="14"/>
+    <tableColumn id="4" name="MIS_MIGRACAO _x000a_201" dataDxfId="13"/>
+    <tableColumn id="5" name="MIS_MIGRACAO _x000a_301" dataDxfId="12"/>
+    <tableColumn id="6" name="MIS_ODS" dataDxfId="11"/>
+    <tableColumn id="7" name="Views _x000a_Oracle" dataDxfId="10"/>
+    <tableColumn id="8" name="SSIS's" dataDxfId="9"/>
+    <tableColumn id="9" name="Data de Correção" dataDxfId="8"/>
+    <tableColumn id="13" name="Observação" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A2:E13" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A2:E13"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Data da Alteração" dataDxfId="6"/>
+    <tableColumn id="2" name="Nome da Tabela/view" dataDxfId="5"/>
+    <tableColumn id="3" name="Nome do Atributo" dataDxfId="4"/>
+    <tableColumn id="4" name="Tipo Alteração" dataDxfId="3"/>
+    <tableColumn id="5" name="Observação" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2749,13 +3001,13 @@
   <sheetData>
     <row r="1" spans="2:4" ht="31.5" customHeight="1">
       <c r="B1" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C1" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="D1" s="29" t="s">
         <v>221</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="2" spans="2:4">
@@ -3056,13 +3308,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M59"/>
+  <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H45" sqref="H45"/>
+      <selection pane="bottomRight" activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -3088,40 +3340,40 @@
         <v>130</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="G1" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="D1" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="G1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="I1" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="I1" s="19" t="s">
-        <v>214</v>
-      </c>
       <c r="J1" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="K1" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="K1" s="19" t="s">
-        <v>205</v>
-      </c>
       <c r="L1" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M1" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -3132,31 +3384,31 @@
         <v>132</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K2" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L2" s="22">
         <v>41876</v>
@@ -3189,31 +3441,31 @@
         <v>132</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L5" s="22">
         <v>41876</v>
@@ -3228,31 +3480,31 @@
         <v>132</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K6" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L6" s="22">
         <v>41876</v>
@@ -3267,31 +3519,31 @@
         <v>132</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K7" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L7" s="22">
         <v>41876</v>
@@ -3324,31 +3576,31 @@
         <v>132</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L10" s="22">
         <v>41876</v>
@@ -3363,31 +3615,31 @@
         <v>132</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L11" s="22">
         <v>41876</v>
@@ -3402,31 +3654,31 @@
         <v>132</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I12" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J12" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K12" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L12" s="22">
         <v>41876</v>
@@ -3441,31 +3693,31 @@
         <v>132</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I13" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L13" s="22">
         <v>41876</v>
@@ -3480,31 +3732,31 @@
         <v>132</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L14" s="22">
         <v>41876</v>
@@ -3519,31 +3771,31 @@
         <v>132</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K15" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L15" s="22">
         <v>41876</v>
@@ -3576,31 +3828,31 @@
         <v>151</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I18" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J18" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K18" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L18" s="22">
         <v>41876</v>
@@ -3615,31 +3867,31 @@
         <v>153</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H19" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I19" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J19" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K19" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L19" s="22">
         <v>41876</v>
@@ -3648,37 +3900,37 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>132</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H20" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I20" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J20" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K20" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L20" s="22">
         <v>41876</v>
@@ -3687,37 +3939,37 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>132</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I21" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J21" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K21" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L21" s="22">
         <v>41876</v>
@@ -3726,37 +3978,37 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>132</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I22" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J22" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L22" s="22">
         <v>41876</v>
@@ -3765,37 +4017,37 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>132</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H23" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I23" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K23" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L23" s="22">
         <v>41876</v>
@@ -3804,37 +4056,37 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="B24" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="B24" s="18" t="s">
-        <v>160</v>
-      </c>
       <c r="C24" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H24" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I24" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K24" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L24" s="22">
         <v>41877</v>
@@ -3843,50 +4095,50 @@
     </row>
     <row r="25" spans="1:13" ht="22.5">
       <c r="A25" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" s="33" t="s">
         <v>161</v>
-      </c>
-      <c r="B25" s="33" t="s">
-        <v>162</v>
       </c>
       <c r="C25" s="34"/>
       <c r="L25" s="20"/>
       <c r="M25" s="32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>132</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H26" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I26" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J26" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K26" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L26" s="22">
         <v>41876</v>
@@ -3895,37 +4147,37 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>132</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H27" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I27" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J27" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K27" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L27" s="22">
         <v>41876</v>
@@ -3934,37 +4186,37 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>132</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H28" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I28" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J28" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K28" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L28" s="22">
         <v>41877</v>
@@ -3973,37 +4225,37 @@
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>132</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H29" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I29" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J29" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K29" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L29" s="22">
         <v>41877</v>
@@ -4012,37 +4264,37 @@
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B30" s="18" t="s">
         <v>132</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G30" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H30" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I30" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J30" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K30" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L30" s="22">
         <v>41877</v>
@@ -4051,37 +4303,37 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="B31" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="B31" s="18" t="s">
-        <v>169</v>
-      </c>
       <c r="C31" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G31" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H31" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I31" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J31" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K31" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L31" s="22">
         <v>41877</v>
@@ -4090,37 +4342,37 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B32" s="18" t="s">
         <v>132</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H32" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I32" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J32" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K32" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L32" s="22">
         <v>41877</v>
@@ -4129,37 +4381,37 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>132</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H33" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I33" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J33" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K33" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L33" s="22">
         <v>41877</v>
@@ -4168,109 +4420,109 @@
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B34" s="21" t="s">
         <v>172</v>
-      </c>
-      <c r="B34" s="21" t="s">
-        <v>173</v>
       </c>
       <c r="M34" s="24"/>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M35" s="24"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M36" s="24"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M37" s="24"/>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M38" s="24"/>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M39" s="24"/>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M40" s="24"/>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B41" s="21" t="s">
         <v>180</v>
-      </c>
-      <c r="B41" s="21" t="s">
-        <v>181</v>
       </c>
       <c r="M41" s="24"/>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="B42" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="B42" s="18" t="s">
-        <v>183</v>
-      </c>
       <c r="C42" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E42" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G42" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H42" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I42" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J42" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K42" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L42" s="22">
         <v>41877</v>
@@ -4279,37 +4531,37 @@
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G43" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H43" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I43" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J43" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K43" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L43" s="22">
         <v>41877</v>
@@ -4317,20 +4569,80 @@
       <c r="M43" s="24"/>
     </row>
     <row r="44" spans="1:13">
-      <c r="A44" s="21" t="s">
+      <c r="A44" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="E44" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="F44" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="G44" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="H44" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="I44" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="J44" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="K44" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="L44" s="22">
+        <v>41880</v>
+      </c>
+      <c r="M44" s="24"/>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="B44" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="M44" s="24"/>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="A45" s="21" t="s">
-        <v>185</v>
-      </c>
-      <c r="B45" s="21" t="s">
-        <v>154</v>
+      <c r="B45" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="E45" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="F45" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="G45" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="H45" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="I45" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="J45" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="K45" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="L45" s="22">
+        <v>41877</v>
       </c>
       <c r="M45" s="24"/>
     </row>
@@ -4342,31 +4654,31 @@
         <v>132</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E46" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F46" s="20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G46" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H46" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I46" s="20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J46" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K46" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L46" s="22">
         <v>41877</v>
@@ -4381,31 +4693,31 @@
         <v>132</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G47" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H47" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I47" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J47" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K47" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L47" s="22">
         <v>41877</v>
@@ -4420,31 +4732,31 @@
         <v>132</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E48" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G48" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H48" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I48" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J48" s="20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="K48" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L48" s="22">
         <v>41877</v>
@@ -4456,34 +4768,34 @@
         <v>189</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>132</v>
+        <v>190</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E49" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G49" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H49" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I49" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J49" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K49" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L49" s="22">
         <v>41877</v>
@@ -4492,37 +4804,37 @@
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="18" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>191</v>
+        <v>132</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E50" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G50" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H50" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I50" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J50" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K50" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L50" s="22">
         <v>41877</v>
@@ -4534,34 +4846,34 @@
         <v>192</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>132</v>
+        <v>193</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E51" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F51" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G51" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H51" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I51" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J51" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K51" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L51" s="22">
         <v>41877</v>
@@ -4570,28 +4882,28 @@
     </row>
     <row r="52" spans="1:13">
       <c r="A52" s="18" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>194</v>
+        <v>132</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E52" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F52" s="20" t="s">
         <v>207</v>
       </c>
       <c r="G52" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H52" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I52" s="20" t="s">
         <v>207</v>
@@ -4600,7 +4912,7 @@
         <v>207</v>
       </c>
       <c r="K52" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L52" s="22">
         <v>41877</v>
@@ -4615,31 +4927,31 @@
         <v>132</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D53" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E53" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F53" s="20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G53" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H53" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I53" s="20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J53" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K53" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L53" s="22">
         <v>41877</v>
@@ -4647,82 +4959,82 @@
       <c r="M53" s="24"/>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="18" t="s">
+      <c r="A54" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="B54" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="C54" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="D54" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="E54" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="F54" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="G54" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="H54" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="I54" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="J54" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="K54" s="20" t="s">
-        <v>207</v>
+      <c r="B54" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="C54" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="D54" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="E54" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="F54" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="G54" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="H54" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="I54" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="J54" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="K54" s="26" t="s">
+        <v>206</v>
       </c>
       <c r="L54" s="22">
         <v>41877</v>
       </c>
-      <c r="M54" s="24"/>
+      <c r="M54" s="27"/>
     </row>
     <row r="55" spans="1:13">
-      <c r="A55" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="B55" s="25" t="s">
+      <c r="A55" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="C55" s="25" t="s">
-        <v>206</v>
-      </c>
-      <c r="D55" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="E55" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="F55" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="G55" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="H55" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="I55" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="J55" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="K55" s="26" t="s">
-        <v>207</v>
+      <c r="B55" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="D55" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="E55" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="F55" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="G55" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="H55" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="I55" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="J55" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="K55" s="20" t="s">
+        <v>206</v>
       </c>
       <c r="L55" s="22">
         <v>41877</v>
       </c>
-      <c r="M55" s="27"/>
+      <c r="M55" s="24"/>
     </row>
     <row r="56" spans="1:13">
       <c r="A56" s="18" t="s">
@@ -4732,36 +5044,38 @@
         <v>132</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E56" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G56" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H56" s="20" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="I56" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J56" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K56" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L56" s="22">
         <v>41877</v>
       </c>
-      <c r="M56" s="24"/>
+      <c r="M56" s="35" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="57" spans="1:13">
       <c r="A57" s="18" t="s">
@@ -4771,116 +5085,390 @@
         <v>132</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E57" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F57" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G57" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H57" s="20" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="I57" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J57" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K57" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L57" s="22">
         <v>41877</v>
       </c>
-      <c r="M57" s="35" t="s">
-        <v>219</v>
-      </c>
+      <c r="M57" s="24"/>
     </row>
     <row r="58" spans="1:13">
       <c r="A58" s="18" t="s">
         <v>201</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>132</v>
+        <v>202</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D58" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E58" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F58" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G58" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H58" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I58" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J58" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K58" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L58" s="22">
         <v>41877</v>
       </c>
       <c r="M58" s="24"/>
     </row>
-    <row r="59" spans="1:13">
-      <c r="A59" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="B59" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="C59" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="D59" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="E59" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="F59" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="G59" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="H59" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="I59" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="J59" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="K59" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="L59" s="22">
-        <v>41877</v>
-      </c>
-      <c r="M59" s="24"/>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:L48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" style="37" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" style="36" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" style="36" customWidth="1"/>
+    <col min="4" max="4" width="47.140625" style="36" customWidth="1"/>
+    <col min="5" max="5" width="43.140625" style="37" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" style="37" customWidth="1"/>
+    <col min="7" max="11" width="9.140625" style="37"/>
+    <col min="12" max="12" width="9.140625" style="38"/>
+    <col min="13" max="16384" width="9.140625" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5">
+      <c r="A2" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>224</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>225</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="39">
+        <v>41880</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>226</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>245</v>
+      </c>
+      <c r="E3" s="40"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="39">
+        <v>41880</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>245</v>
+      </c>
+      <c r="E4" s="40"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="39">
+        <v>41880</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="E5" s="40"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="39">
+        <v>41880</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>233</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>247</v>
+      </c>
+      <c r="E6" s="40"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="39">
+        <v>41880</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>237</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="E7" s="40"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="39">
+        <v>41880</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>238</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="E8" s="40"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="39">
+        <v>41880</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="E9" s="40"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="43">
+        <v>41880</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>240</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>205</v>
+      </c>
+      <c r="D10" s="46" t="s">
+        <v>249</v>
+      </c>
+      <c r="E10" s="45"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="43">
+        <v>41880</v>
+      </c>
+      <c r="B11" s="46" t="s">
+        <v>241</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>242</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>244</v>
+      </c>
+      <c r="E11" s="45"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="43">
+        <v>41880</v>
+      </c>
+      <c r="B12" s="46" t="s">
+        <v>241</v>
+      </c>
+      <c r="C12" s="46" t="s">
+        <v>243</v>
+      </c>
+      <c r="D12" s="46" t="s">
+        <v>244</v>
+      </c>
+      <c r="E12" s="40"/>
+    </row>
+    <row r="13" spans="1:5" ht="51">
+      <c r="A13" s="39">
+        <v>41880</v>
+      </c>
+      <c r="B13" s="42" t="s">
+        <v>234</v>
+      </c>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="41" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="E14" s="40"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="E15" s="40"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="E16" s="40"/>
+    </row>
+    <row r="17" spans="5:5">
+      <c r="E17" s="40"/>
+    </row>
+    <row r="18" spans="5:5">
+      <c r="E18" s="40"/>
+    </row>
+    <row r="19" spans="5:5">
+      <c r="E19" s="40"/>
+    </row>
+    <row r="20" spans="5:5">
+      <c r="E20" s="40"/>
+    </row>
+    <row r="21" spans="5:5">
+      <c r="E21" s="40"/>
+    </row>
+    <row r="22" spans="5:5">
+      <c r="E22" s="40"/>
+    </row>
+    <row r="23" spans="5:5">
+      <c r="E23" s="40"/>
+    </row>
+    <row r="24" spans="5:5">
+      <c r="E24" s="40"/>
+    </row>
+    <row r="25" spans="5:5">
+      <c r="E25" s="40"/>
+    </row>
+    <row r="26" spans="5:5">
+      <c r="E26" s="40"/>
+    </row>
+    <row r="27" spans="5:5">
+      <c r="E27" s="40"/>
+    </row>
+    <row r="28" spans="5:5">
+      <c r="E28" s="40"/>
+    </row>
+    <row r="29" spans="5:5">
+      <c r="E29" s="40"/>
+    </row>
+    <row r="30" spans="5:5">
+      <c r="E30" s="40"/>
+    </row>
+    <row r="31" spans="5:5">
+      <c r="E31" s="40"/>
+    </row>
+    <row r="32" spans="5:5">
+      <c r="E32" s="40"/>
+    </row>
+    <row r="33" spans="5:5">
+      <c r="E33" s="40"/>
+    </row>
+    <row r="34" spans="5:5">
+      <c r="E34" s="40"/>
+    </row>
+    <row r="35" spans="5:5">
+      <c r="E35" s="40"/>
+    </row>
+    <row r="36" spans="5:5">
+      <c r="E36" s="40"/>
+    </row>
+    <row r="37" spans="5:5">
+      <c r="E37" s="40"/>
+    </row>
+    <row r="38" spans="5:5">
+      <c r="E38" s="40"/>
+    </row>
+    <row r="39" spans="5:5">
+      <c r="E39" s="40"/>
+    </row>
+    <row r="40" spans="5:5">
+      <c r="E40" s="40"/>
+    </row>
+    <row r="41" spans="5:5">
+      <c r="E41" s="40"/>
+    </row>
+    <row r="42" spans="5:5">
+      <c r="E42" s="40"/>
+    </row>
+    <row r="43" spans="5:5">
+      <c r="E43" s="40"/>
+    </row>
+    <row r="44" spans="5:5">
+      <c r="E44" s="40"/>
+    </row>
+    <row r="45" spans="5:5">
+      <c r="E45" s="40"/>
+    </row>
+    <row r="46" spans="5:5">
+      <c r="E46" s="40"/>
+    </row>
+    <row r="47" spans="5:5">
+      <c r="E47" s="40"/>
+    </row>
+    <row r="48" spans="5:5">
+      <c r="E48" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Atualização de Documentação ODS e LN
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Controle_Alteracao.xlsx
+++ b/Documentação/Planilhas/Controle_Alteracao.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="277">
   <si>
     <t>RESPONSÁVEL</t>
   </si>
@@ -829,6 +829,30 @@
   </si>
   <si>
     <t>NR_CONTA</t>
+  </si>
+  <si>
+    <t>correção na view</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>301</t>
+  </si>
+  <si>
+    <t>Correção das despesas e impostos</t>
+  </si>
+  <si>
+    <t>Mostrar ref fiscal de remessa quando fatura e correções do rateio de juros</t>
+  </si>
+  <si>
+    <t>vw_wms_volumetria</t>
+  </si>
+  <si>
+    <t>correção encaminhada pelo Riccardo</t>
+  </si>
+  <si>
+    <t>correção na view [feito apenas no criciuma01 (201 e 301)]</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +1024,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1108,11 +1132,66 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1514,7 +1593,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A1:M58" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A1:M58" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A1:M58">
     <filterColumn colId="3"/>
     <filterColumn colId="4"/>
@@ -1522,33 +1601,38 @@
     <filterColumn colId="12"/>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" name="tabela" dataDxfId="19"/>
-    <tableColumn id="2" name="nome_campo_x000a_ (DE)" dataDxfId="18"/>
-    <tableColumn id="3" name="nome_campo0 _x000a_(PARA)" dataDxfId="17"/>
-    <tableColumn id="12" name="GitHub" dataDxfId="16"/>
-    <tableColumn id="10" name="Mapeamento_Stage_LN" dataDxfId="15"/>
-    <tableColumn id="11" name="Mapeamento_ODS_LN" dataDxfId="14"/>
-    <tableColumn id="4" name="MIS_MIGRACAO _x000a_201" dataDxfId="13"/>
-    <tableColumn id="5" name="MIS_MIGRACAO _x000a_301" dataDxfId="12"/>
-    <tableColumn id="6" name="MIS_ODS" dataDxfId="11"/>
-    <tableColumn id="7" name="Views _x000a_Oracle" dataDxfId="10"/>
-    <tableColumn id="8" name="SSIS's" dataDxfId="9"/>
-    <tableColumn id="9" name="Data de Correção" dataDxfId="8"/>
-    <tableColumn id="13" name="Observação" dataDxfId="7"/>
+    <tableColumn id="1" name="tabela" dataDxfId="21"/>
+    <tableColumn id="2" name="nome_campo_x000a_ (DE)" dataDxfId="20"/>
+    <tableColumn id="3" name="nome_campo0 _x000a_(PARA)" dataDxfId="19"/>
+    <tableColumn id="12" name="GitHub" dataDxfId="18"/>
+    <tableColumn id="10" name="Mapeamento_Stage_LN" dataDxfId="17"/>
+    <tableColumn id="11" name="Mapeamento_ODS_LN" dataDxfId="16"/>
+    <tableColumn id="4" name="MIS_MIGRACAO _x000a_201" dataDxfId="15"/>
+    <tableColumn id="5" name="MIS_MIGRACAO _x000a_301" dataDxfId="14"/>
+    <tableColumn id="6" name="MIS_ODS" dataDxfId="13"/>
+    <tableColumn id="7" name="Views _x000a_Oracle" dataDxfId="12"/>
+    <tableColumn id="8" name="SSIS's" dataDxfId="11"/>
+    <tableColumn id="9" name="Data de Correção" dataDxfId="10"/>
+    <tableColumn id="13" name="Observação" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A2:E27" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A2:E27"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Data da Alteração" dataDxfId="4"/>
-    <tableColumn id="2" name="Nome da Tabela/view" dataDxfId="3"/>
-    <tableColumn id="3" name="Nome do Atributo" dataDxfId="2"/>
-    <tableColumn id="4" name="Tipo Alteração" dataDxfId="1"/>
-    <tableColumn id="5" name="Observação" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A2:G30" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A2:G30">
+    <filterColumn colId="5"/>
+    <filterColumn colId="6"/>
+  </autoFilter>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Data da Alteração" dataDxfId="6"/>
+    <tableColumn id="2" name="Nome da Tabela/view" dataDxfId="5"/>
+    <tableColumn id="3" name="Nome do Atributo" dataDxfId="4"/>
+    <tableColumn id="4" name="Tipo Alteração" dataDxfId="3"/>
+    <tableColumn id="5" name="Observação" dataDxfId="2"/>
+    <tableColumn id="6" name="201" dataDxfId="1"/>
+    <tableColumn id="7" name="301" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5229,8 +5313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5240,13 +5324,13 @@
     <col min="3" max="3" width="26.85546875" style="36" customWidth="1"/>
     <col min="4" max="4" width="47.140625" style="36" customWidth="1"/>
     <col min="5" max="5" width="43.140625" style="37" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" style="37" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="37" customWidth="1"/>
     <col min="7" max="11" width="9.140625" style="37"/>
     <col min="12" max="12" width="9.140625" style="38"/>
     <col min="13" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" s="37" t="s">
         <v>230</v>
       </c>
@@ -5262,8 +5346,14 @@
       <c r="E2" s="37" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="49" t="s">
+        <v>270</v>
+      </c>
+      <c r="G2" s="49" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="39">
         <v>41880</v>
       </c>
@@ -5277,8 +5367,10 @@
         <v>245</v>
       </c>
       <c r="E3" s="40"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="39">
         <v>41880</v>
       </c>
@@ -5292,8 +5384,10 @@
         <v>245</v>
       </c>
       <c r="E4" s="40"/>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="39">
         <v>41880</v>
       </c>
@@ -5307,8 +5401,10 @@
         <v>246</v>
       </c>
       <c r="E5" s="40"/>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="39">
         <v>41880</v>
       </c>
@@ -5322,8 +5418,10 @@
         <v>247</v>
       </c>
       <c r="E6" s="40"/>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="39">
         <v>41880</v>
       </c>
@@ -5337,8 +5435,10 @@
         <v>248</v>
       </c>
       <c r="E7" s="40"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="39">
         <v>41880</v>
       </c>
@@ -5352,8 +5452,10 @@
         <v>248</v>
       </c>
       <c r="E8" s="40"/>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="39">
         <v>41880</v>
       </c>
@@ -5367,8 +5469,10 @@
         <v>248</v>
       </c>
       <c r="E9" s="40"/>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="43">
         <v>41880</v>
       </c>
@@ -5382,8 +5486,14 @@
         <v>249</v>
       </c>
       <c r="E10" s="45"/>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="43">
         <v>41880</v>
       </c>
@@ -5397,8 +5507,10 @@
         <v>244</v>
       </c>
       <c r="E11" s="45"/>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="43">
         <v>41880</v>
       </c>
@@ -5412,8 +5524,10 @@
         <v>244</v>
       </c>
       <c r="E12" s="40"/>
-    </row>
-    <row r="13" spans="1:5" ht="51">
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+    </row>
+    <row r="13" spans="1:7" ht="51">
       <c r="A13" s="39">
         <v>41880</v>
       </c>
@@ -5425,8 +5539,10 @@
       <c r="E13" s="41" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="43">
         <v>41883</v>
       </c>
@@ -5440,8 +5556,10 @@
         <v>251</v>
       </c>
       <c r="E14" s="45"/>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="43">
         <v>41883</v>
       </c>
@@ -5455,8 +5573,10 @@
         <v>251</v>
       </c>
       <c r="E15" s="48"/>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="43">
         <v>41883</v>
       </c>
@@ -5470,8 +5590,10 @@
         <v>251</v>
       </c>
       <c r="E16" s="48"/>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="43">
         <v>41883</v>
       </c>
@@ -5485,8 +5607,10 @@
         <v>251</v>
       </c>
       <c r="E17" s="48"/>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="43">
         <v>41883</v>
       </c>
@@ -5500,8 +5624,10 @@
         <v>251</v>
       </c>
       <c r="E18" s="48"/>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="43">
         <v>41883</v>
       </c>
@@ -5515,8 +5641,10 @@
         <v>251</v>
       </c>
       <c r="E19" s="48"/>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="43">
         <v>41883</v>
       </c>
@@ -5530,8 +5658,14 @@
         <v>249</v>
       </c>
       <c r="E20" s="45"/>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="43">
         <v>41883</v>
       </c>
@@ -5545,8 +5679,14 @@
         <v>249</v>
       </c>
       <c r="E21" s="45"/>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="43">
         <v>41883</v>
       </c>
@@ -5560,8 +5700,14 @@
         <v>249</v>
       </c>
       <c r="E22" s="45"/>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="43">
         <v>41883</v>
       </c>
@@ -5577,8 +5723,14 @@
       <c r="E23" s="45" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="43">
         <v>41883</v>
       </c>
@@ -5586,12 +5738,20 @@
         <v>263</v>
       </c>
       <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
+      <c r="D24" s="44" t="s">
+        <v>269</v>
+      </c>
       <c r="E24" s="45" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="43">
         <v>41883</v>
       </c>
@@ -5605,8 +5765,10 @@
         <v>249</v>
       </c>
       <c r="E25" s="48"/>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="43">
         <v>41883</v>
       </c>
@@ -5620,8 +5782,10 @@
         <v>249</v>
       </c>
       <c r="E26" s="48"/>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="43">
         <v>41883</v>
       </c>
@@ -5635,20 +5799,70 @@
         <v>249</v>
       </c>
       <c r="E27" s="48"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="E28" s="40"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="E29" s="40"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="E30" s="40"/>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+    </row>
+    <row r="28" spans="1:7" ht="25.5">
+      <c r="A28" s="43">
+        <v>41884</v>
+      </c>
+      <c r="B28" s="53" t="s">
+        <v>263</v>
+      </c>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53" t="s">
+        <v>269</v>
+      </c>
+      <c r="E28" s="52" t="s">
+        <v>273</v>
+      </c>
+      <c r="F28" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="43"/>
+      <c r="B29" s="44" t="s">
+        <v>261</v>
+      </c>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="E29" s="45" t="s">
+        <v>272</v>
+      </c>
+      <c r="F29" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="G29" s="50" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="54"/>
+      <c r="B30" s="46" t="s">
+        <v>274</v>
+      </c>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46" t="s">
+        <v>276</v>
+      </c>
+      <c r="E30" s="51" t="s">
+        <v>275</v>
+      </c>
+      <c r="F30" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="55"/>
+    </row>
+    <row r="31" spans="1:7">
       <c r="E31" s="40"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:7">
       <c r="E32" s="40"/>
     </row>
     <row r="33" spans="5:5">

</xml_diff>

<commit_message>
Documentação Controle de Alteração
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Controle_Alteracao.xlsx
+++ b/Documentação/Planilhas/Controle_Alteracao.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="303">
   <si>
     <t>RESPONSÁVEL</t>
   </si>
@@ -930,6 +930,9 @@
   </si>
   <si>
     <t>FAT_FATURAMENTO</t>
+  </si>
+  <si>
+    <t>inclusão do to_char no CD_MEIO_PAGAMENTO_PRINCIPAL</t>
   </si>
 </sst>
 </file>
@@ -1294,7 +1297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1462,6 +1465,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1936,8 +1942,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A2:G31" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A2:G31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A2:G32" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A2:G32">
     <filterColumn colId="5"/>
     <filterColumn colId="6"/>
   </autoFilter>
@@ -5642,7 +5648,7 @@
   <dimension ref="A2:L48"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6210,8 +6216,26 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
-      <c r="E32" s="40"/>
+    <row r="32" spans="1:7" ht="25.5">
+      <c r="A32" s="43">
+        <v>41890</v>
+      </c>
+      <c r="B32" s="53" t="s">
+        <v>228</v>
+      </c>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53" t="s">
+        <v>269</v>
+      </c>
+      <c r="E32" s="70" t="s">
+        <v>302</v>
+      </c>
+      <c r="F32" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="50" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="33" spans="5:5">
       <c r="E33" s="40"/>
@@ -6442,7 +6466,7 @@
   <dimension ref="A2:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:E4"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6612,24 +6636,60 @@
       <c r="A5" s="55">
         <v>41890</v>
       </c>
-      <c r="B5" s="62"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="63"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="63"/>
-      <c r="N5" s="62"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="63"/>
-      <c r="R5" s="62"/>
-      <c r="S5" s="63"/>
+      <c r="B5" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="I5" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="L5" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="M5" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="N5" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="O5" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="P5" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q5" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="R5" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="S5" s="63" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="55">

</xml_diff>

<commit_message>
Atualização controle atualização VIEWS
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Controle_Alteracao.xlsx
+++ b/Documentação/Planilhas/Controle_Alteracao.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="timezone" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="310">
   <si>
     <t>RESPONSÁVEL</t>
   </si>
@@ -948,6 +948,12 @@
   </si>
   <si>
     <t>Fiz em 10/09 pela manhã</t>
+  </si>
+  <si>
+    <t>Correção do relacionamento com a ordem de venda</t>
+  </si>
+  <si>
+    <t>Alterado somente no ambiente 201</t>
   </si>
 </sst>
 </file>
@@ -1960,8 +1966,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A2:G35" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A2:G35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A2:G36" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A2:G36">
     <filterColumn colId="5"/>
     <filterColumn colId="6"/>
   </autoFilter>
@@ -5665,8 +5671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:L48"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6307,7 +6313,23 @@
       <c r="G35" s="49"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="E36" s="40"/>
+      <c r="A36" s="43">
+        <v>41911</v>
+      </c>
+      <c r="B36" s="44" t="s">
+        <v>241</v>
+      </c>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44" t="s">
+        <v>308</v>
+      </c>
+      <c r="E36" s="45" t="s">
+        <v>309</v>
+      </c>
+      <c r="F36" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="G36" s="50"/>
     </row>
     <row r="37" spans="1:7">
       <c r="E37" s="40"/>
@@ -6525,7 +6547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15:H16"/>
     </sheetView>
   </sheetViews>

</xml_diff>